<commit_message>
[Feat] Equipment Mannage resolucion de observaciones  y a qa
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/equipment/EquipmentFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/equipment/EquipmentFormulario.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\workspace\axsis\LabRamos\API\Service.Catalog\wwwroot\layout\excel\equipment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70FC034-5294-41C5-9876-6B61AE53A518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01A3F69-5155-49FD-A3B7-1A7EE42BDDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sucursales" sheetId="1" r:id="rId1"/>
+    <sheet name="Equipos" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Sucursales" localSheetId="0">Sucursales!$A$3:$F$19</definedName>
+    <definedName name="Sucursales" localSheetId="0">Equipos!$A$3:$F$19</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -176,14 +176,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,11 +566,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
@@ -614,7 +614,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="6"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -708,11 +708,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:F11"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="A1:C1"/>
@@ -723,6 +718,11 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
[Fix] Equipment - update, print, download, acces to views
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/equipment/EquipmentFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/equipment/EquipmentFormulario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\workspace\axsis\LabRamos\API\Service.Catalog\wwwroot\layout\excel\equipment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01A3F69-5155-49FD-A3B7-1A7EE42BDDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63382755-C81E-4D01-8DBF-A4C110843D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Equipos" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Sucursales" localSheetId="0">Equipos!$A$3:$F$19</definedName>
+    <definedName name="Valores" localSheetId="0">Equipos!$A$8:$B$9</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Clave</t>
   </si>
@@ -78,19 +78,31 @@
     <t>Activo</t>
   </si>
   <si>
-    <t>{{Sucursales.Clave}}</t>
-  </si>
-  <si>
-    <t>{{Sucursales.Nombre}}</t>
-  </si>
-  <si>
-    <t>{{Sucursales.Activo}}</t>
-  </si>
-  <si>
-    <t>{{Sucursales.Categoria}}</t>
-  </si>
-  <si>
     <t>Categoría</t>
+  </si>
+  <si>
+    <t>Sucursal</t>
+  </si>
+  <si>
+    <t>{{Equipos.Clave}}</t>
+  </si>
+  <si>
+    <t>{{Equipos.Nombre}}</t>
+  </si>
+  <si>
+    <t>{{Equipos.Activo}}</t>
+  </si>
+  <si>
+    <t>{{item.Num_Serie}}</t>
+  </si>
+  <si>
+    <t>{{Equipos.CategoriaText}}</t>
+  </si>
+  <si>
+    <t>{{item.SucursalText}}</t>
+  </si>
+  <si>
+    <t>Número de Serie</t>
   </si>
 </sst>
 </file>
@@ -165,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -178,6 +190,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -554,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8A4281-45E9-4A26-88B5-8DB32AE336F4}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,11 +587,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
@@ -578,17 +599,17 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="5"/>
+      <c r="E3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -599,17 +620,17 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="5"/>
+      <c r="B5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8"/>
       <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="5"/>
+      <c r="E5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -617,112 +638,197 @@
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="A7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
       <c r="D10" s="1"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="6"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="C17" s="3"/>
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="6"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="C19" s="3"/>
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="5">
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B13:C13"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E9:F9"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>